<commit_message>
2020-06-11 13:59, latest updates, using Python to commit
</commit_message>
<xml_diff>
--- a/_notProduction/tools/excel/formulas.xlsx
+++ b/_notProduction/tools/excel/formulas.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnaylor\Desktop\portableProcedures\repos\publicProjects\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\creed\repos\publicProjects\_notProduction\tools\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CA8C1B-CC28-46D9-9FEA-4CD6C56F4311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D509DE6-DAD3-4AD2-83D0-B5CC62FF925E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29E67950-BA9F-48E6-A89A-0FBE7B506AEB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29E67950-BA9F-48E6-A89A-0FBE7B506AEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Excel" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -405,7 +407,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2020-07-06 11:30, latest updates, using Python to commit
</commit_message>
<xml_diff>
--- a/_notProduction/tools/excel/formulas.xlsx
+++ b/_notProduction/tools/excel/formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\creed\repos\publicProjects\_notProduction\tools\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D509DE6-DAD3-4AD2-83D0-B5CC62FF925E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BA3636-FC60-4BBC-BF83-464FA5BC8C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29E67950-BA9F-48E6-A89A-0FBE7B506AEB}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>